<commit_message>
[FIX] commit before cleaning
</commit_message>
<xml_diff>
--- a/data/Biomass_composition.xlsx
+++ b/data/Biomass_composition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bisbii\PythonProjects\model_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2491AFBC-CF43-4854-9218-0A93E3FED037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB8CE9B-DDB5-4382-A067-746493E8B842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Macromolecular Composition" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="535">
   <si>
     <t>g/gDCW</t>
   </si>
@@ -1686,6 +1686,12 @@
   </si>
   <si>
     <t>g/gDW2</t>
+  </si>
+  <si>
+    <t>max carbs</t>
+  </si>
+  <si>
+    <t>soluble</t>
   </si>
 </sst>
 </file>
@@ -2310,15 +2316,6 @@
   </cellStyles>
   <dxfs count="41">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="166" formatCode="0.00000"/>
     </dxf>
     <dxf>
@@ -2344,6 +2341,15 @@
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2699,8 +2705,8 @@
     <tableColumn id="4" xr3:uid="{559CC120-24BE-4374-8E79-D1B44B0CFAA3}" name="Reduced MW"/>
     <tableColumn id="5" xr3:uid="{7F8E2606-94C5-49F5-A463-001394855063}" name="mol/mole-Cofactor"/>
     <tableColumn id="6" xr3:uid="{DEF98CF4-ACAE-4C1F-B46A-C03C499FEF97}" name="gmetabolite/ge-Cofactor"/>
-    <tableColumn id="7" xr3:uid="{F3550C60-2C03-40AE-B65C-CF9C869929FA}" name="mmolmetabolite/ge-Cofactor" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{8A9553C4-02C7-4839-8445-47C770CF3BF0}" name="gmetabolite/gDW" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{F3550C60-2C03-40AE-B65C-CF9C869929FA}" name="mmolmetabolite/ge-Cofactor" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{8A9553C4-02C7-4839-8445-47C770CF3BF0}" name="gmetabolite/gDW" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2837,13 +2843,13 @@
     <tableColumn id="20" xr3:uid="{5321F775-DCFA-4809-9AFA-C0BD62C17388}" name="mg/gMM" dataDxfId="8">
       <calculatedColumnFormula>Table7[[#This Row],[mmol M/ gMM]]*Table7[[#This Row],[Mol.Weight]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{70C9B5B8-88CC-4C4F-8DEA-C1491A61CCEC}" name="g/gDW2" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{70C9B5B8-88CC-4C4F-8DEA-C1491A61CCEC}" name="g/gDW2" dataDxfId="7">
       <calculatedColumnFormula>Table7[[#This Row],[g/gDW]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E86A0115-F2DE-4234-9A19-AAC6F53B8B57}" name="gM/gMM" dataDxfId="1">
+    <tableColumn id="7" xr3:uid="{E86A0115-F2DE-4234-9A19-AAC6F53B8B57}" name="gM/gMM" dataDxfId="6">
       <calculatedColumnFormula>Table7[[#This Row],[g/gDW2]]/$R$12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{8A438586-5B82-4DC7-8BFD-5A492222E39C}" name="mmolM/gMM" dataDxfId="0">
+    <tableColumn id="11" xr3:uid="{8A438586-5B82-4DC7-8BFD-5A492222E39C}" name="mmolM/gMM" dataDxfId="5">
       <calculatedColumnFormula>Table7[[#This Row],[gM/gMM]]/Table7[[#This Row],[Mol.Weight]]*1000</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2861,9 +2867,9 @@
     <tableColumn id="4" xr3:uid="{EFBCA1AC-A49B-4835-BD8F-C8ED24318EE4}" name="% (molar)"/>
     <tableColumn id="5" xr3:uid="{138F6833-EFF1-4489-B8B7-8F8801BB08A1}" name="mol M / mol MM"/>
     <tableColumn id="6" xr3:uid="{BCCBBB05-F485-482F-977D-E22C1F9171AC}" name="g/molM"/>
-    <tableColumn id="7" xr3:uid="{2D0ED677-49CD-4530-A4CB-8E854404F4F3}" name="mmol M/gMM" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{76A3A56E-B60B-45B3-AC1C-E55732BF706D}" name="mmol M/ gDW" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{1F5BDFF6-2905-47F5-BBCA-6E3683E465AC}" name="g/gDW" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{2D0ED677-49CD-4530-A4CB-8E854404F4F3}" name="mmol M/gMM" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{76A3A56E-B60B-45B3-AC1C-E55732BF706D}" name="mmol M/ gDW" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{1F5BDFF6-2905-47F5-BBCA-6E3683E465AC}" name="g/gDW" dataDxfId="2"/>
     <tableColumn id="10" xr3:uid="{38BD67F6-8E61-4B5A-B82D-F86A841ACE6C}" name="Column2">
       <calculatedColumnFormula>L8*1000</calculatedColumnFormula>
     </tableColumn>
@@ -3138,7 +3144,7 @@
   <dimension ref="B3:L48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6527,12 +6533,42 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="I6:I17"/>
-    <mergeCell ref="B6:B17"/>
-    <mergeCell ref="E6:E17"/>
-    <mergeCell ref="F6:F17"/>
-    <mergeCell ref="G6:G17"/>
-    <mergeCell ref="H6:H17"/>
+    <mergeCell ref="I67:I90"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="E63:E66"/>
+    <mergeCell ref="F63:F66"/>
+    <mergeCell ref="G63:G66"/>
+    <mergeCell ref="H63:H66"/>
+    <mergeCell ref="I63:I66"/>
+    <mergeCell ref="B67:B90"/>
+    <mergeCell ref="E67:E90"/>
+    <mergeCell ref="F67:F90"/>
+    <mergeCell ref="G67:G90"/>
+    <mergeCell ref="H67:H90"/>
+    <mergeCell ref="I59:I62"/>
+    <mergeCell ref="B39:B58"/>
+    <mergeCell ref="E39:E58"/>
+    <mergeCell ref="F39:F58"/>
+    <mergeCell ref="G39:G58"/>
+    <mergeCell ref="H39:H58"/>
+    <mergeCell ref="I39:I58"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="E59:E62"/>
+    <mergeCell ref="F59:F62"/>
+    <mergeCell ref="G59:G62"/>
+    <mergeCell ref="H59:H62"/>
+    <mergeCell ref="I34:I38"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="F30:F33"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="I30:I33"/>
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="E34:E38"/>
+    <mergeCell ref="F34:F38"/>
+    <mergeCell ref="G34:G38"/>
+    <mergeCell ref="H34:H38"/>
     <mergeCell ref="I22:I29"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="E18:E21"/>
@@ -6545,42 +6581,12 @@
     <mergeCell ref="F22:F29"/>
     <mergeCell ref="G22:G29"/>
     <mergeCell ref="H22:H29"/>
-    <mergeCell ref="I34:I38"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="F30:F33"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="I30:I33"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="E34:E38"/>
-    <mergeCell ref="F34:F38"/>
-    <mergeCell ref="G34:G38"/>
-    <mergeCell ref="H34:H38"/>
-    <mergeCell ref="I59:I62"/>
-    <mergeCell ref="B39:B58"/>
-    <mergeCell ref="E39:E58"/>
-    <mergeCell ref="F39:F58"/>
-    <mergeCell ref="G39:G58"/>
-    <mergeCell ref="H39:H58"/>
-    <mergeCell ref="I39:I58"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="E59:E62"/>
-    <mergeCell ref="F59:F62"/>
-    <mergeCell ref="G59:G62"/>
-    <mergeCell ref="H59:H62"/>
-    <mergeCell ref="I67:I90"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="E63:E66"/>
-    <mergeCell ref="F63:F66"/>
-    <mergeCell ref="G63:G66"/>
-    <mergeCell ref="H63:H66"/>
-    <mergeCell ref="I63:I66"/>
-    <mergeCell ref="B67:B90"/>
-    <mergeCell ref="E67:E90"/>
-    <mergeCell ref="F67:F90"/>
-    <mergeCell ref="G67:G90"/>
-    <mergeCell ref="H67:H90"/>
+    <mergeCell ref="I6:I17"/>
+    <mergeCell ref="B6:B17"/>
+    <mergeCell ref="E6:E17"/>
+    <mergeCell ref="F6:F17"/>
+    <mergeCell ref="G6:G17"/>
+    <mergeCell ref="H6:H17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8482,7 +8488,7 @@
   <dimension ref="C1:AL222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -8637,6 +8643,10 @@
         <f>O4*'Macromolecular Composition'!$H$7</f>
         <v>1.3057017931404239E-2</v>
       </c>
+      <c r="T4" s="8">
+        <f>0.2-R16+Table8[[#This Row],[g M / g DW]]</f>
+        <v>0.10205701793140423</v>
+      </c>
     </row>
     <row r="5" spans="3:30">
       <c r="C5" s="8" t="s">
@@ -8697,6 +8707,10 @@
       <c r="R5" s="8">
         <f>O5*'Macromolecular Composition'!$H$7</f>
         <v>1.0033346912066697E-2</v>
+      </c>
+      <c r="T5" s="8">
+        <f>T4+SUM(R5:R15)</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="6" spans="3:30">
@@ -20427,10 +20441,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3052ACEE-4180-40AA-90A3-9877406B1F04}">
-  <dimension ref="B6:K15"/>
+  <dimension ref="B6:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20714,6 +20728,41 @@
       <c r="J15">
         <f>J11-J9</f>
         <v>2.9832709062364562</v>
+      </c>
+    </row>
+    <row r="19" spans="10:11">
+      <c r="J19" t="s">
+        <v>533</v>
+      </c>
+      <c r="K19">
+        <v>72.739999999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="10:11">
+      <c r="J20" t="s">
+        <v>534</v>
+      </c>
+      <c r="K20">
+        <f>SUM(K7:K8,K10)*100</f>
+        <v>19.78357483980805</v>
+      </c>
+    </row>
+    <row r="21" spans="10:11">
+      <c r="K21">
+        <f>K19-K20</f>
+        <v>52.956425160191941</v>
+      </c>
+    </row>
+    <row r="22" spans="10:11">
+      <c r="K22">
+        <f>K21-K9*100</f>
+        <v>23.239999999999984</v>
+      </c>
+    </row>
+    <row r="23" spans="10:11">
+      <c r="K23">
+        <f>K22/100</f>
+        <v>0.23239999999999983</v>
       </c>
     </row>
   </sheetData>
@@ -20970,8 +21019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B0B1A99-6869-4CA8-8AFF-CDE465AFCC99}">
   <dimension ref="A2:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>